<commit_message>
[ADD] scripts for manual curation
</commit_message>
<xml_diff>
--- a/data/manual_annotations.xlsx
+++ b/data/manual_annotations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baeuerle/Organisation/Masterarbeit/C_striatum_GEMs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{222DB679-06D8-B146-BF90-07C8D9687DA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC2C3167-BE21-8E40-A04E-519281277169}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12440" windowHeight="21600" xr2:uid="{8C7181AF-021E-984D-A4FD-BACD10035A87}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10000" windowHeight="21600" xr2:uid="{8C7181AF-021E-984D-A4FD-BACD10035A87}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -1091,7 +1091,7 @@
   <dimension ref="A1:M66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A67" sqref="A67:XFD67"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
[v6.1] extend metabolite annotation
</commit_message>
<xml_diff>
--- a/data/manual_annotations.xlsx
+++ b/data/manual_annotations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baeuerle/Organisation/Masterarbeit/C_striatum_GEMs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC2C3167-BE21-8E40-A04E-519281277169}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDC9153D-03F8-5F4B-B97A-5A34B428E6AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10000" windowHeight="21600" xr2:uid="{8C7181AF-021E-984D-A4FD-BACD10035A87}"/>
+    <workbookView xWindow="-33600" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{8C7181AF-021E-984D-A4FD-BACD10035A87}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="251">
   <si>
     <t>1ag160</t>
   </si>
@@ -719,6 +719,72 @@
   </si>
   <si>
     <t>CHEBI:73890</t>
+  </si>
+  <si>
+    <t>CHEBI:4224</t>
+  </si>
+  <si>
+    <t>CHEBI:42207</t>
+  </si>
+  <si>
+    <t>CHEBI:13007</t>
+  </si>
+  <si>
+    <t>CHEBI:21067</t>
+  </si>
+  <si>
+    <t>CHEBI:27125</t>
+  </si>
+  <si>
+    <t>CHEBI:15261</t>
+  </si>
+  <si>
+    <t>CHEBI:27127</t>
+  </si>
+  <si>
+    <t>CHEBI:58389</t>
+  </si>
+  <si>
+    <t>CHEBI:9732</t>
+  </si>
+  <si>
+    <t>HMDB00906</t>
+  </si>
+  <si>
+    <t>R-ALL-30373</t>
+  </si>
+  <si>
+    <t>CHEBI:87252</t>
+  </si>
+  <si>
+    <t>HMDB0011564</t>
+  </si>
+  <si>
+    <t>CHEBI:43165</t>
+  </si>
+  <si>
+    <t>CHEBI:11058</t>
+  </si>
+  <si>
+    <t>CHEBI:412</t>
+  </si>
+  <si>
+    <t>CHEBI:18770</t>
+  </si>
+  <si>
+    <t>CHEBI:46051</t>
+  </si>
+  <si>
+    <t>CHEBI:19337</t>
+  </si>
+  <si>
+    <t>CHEBI:8096</t>
+  </si>
+  <si>
+    <t>CHEBI:44780</t>
+  </si>
+  <si>
+    <t>HMDB0012154</t>
   </si>
 </sst>
 </file>
@@ -768,12 +834,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1088,11 +1155,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06681DF7-667C-1E45-B94D-A8C9F37417A3}">
-  <dimension ref="A1:M66"/>
+  <dimension ref="A1:M84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A67" sqref="A67:XFD67"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K86" sqref="K86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1103,49 +1170,49 @@
     <col min="5" max="5" width="15.33203125" customWidth="1"/>
     <col min="7" max="7" width="11.83203125" customWidth="1"/>
     <col min="8" max="9" width="13" customWidth="1"/>
-    <col min="10" max="10" width="13" style="2" customWidth="1"/>
+    <col min="10" max="10" width="13" style="5" customWidth="1"/>
     <col min="11" max="11" width="17" customWidth="1"/>
     <col min="12" max="12" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>183</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="2" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1165,859 +1232,1087 @@
       <c r="E2" t="s">
         <v>98</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2" s="5">
         <v>71567</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>94</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" t="s">
-        <v>31</v>
-      </c>
-      <c r="J3" s="2">
-        <v>5103842</v>
+        <v>229</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>94</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" t="s">
-        <v>52</v>
+        <v>230</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="B5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C5" t="s">
-        <v>115</v>
-      </c>
-      <c r="D5" t="s">
-        <v>118</v>
-      </c>
-      <c r="E5" t="s">
-        <v>119</v>
-      </c>
-      <c r="F5" t="s">
-        <v>116</v>
-      </c>
-      <c r="H5" t="s">
-        <v>117</v>
-      </c>
-      <c r="J5" s="2">
-        <v>1146</v>
-      </c>
-      <c r="M5" t="s">
-        <v>120</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>94</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" t="s">
-        <v>39</v>
-      </c>
-      <c r="J6" s="2">
-        <v>5375469</v>
-      </c>
-      <c r="L6" t="s">
-        <v>36</v>
+        <v>232</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>71</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E7" t="s">
-        <v>74</v>
-      </c>
-      <c r="J7" s="2">
-        <v>56927861</v>
+        <v>31</v>
+      </c>
+      <c r="J7" s="5">
+        <v>5103842</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s">
-        <v>77</v>
+        <v>51</v>
       </c>
       <c r="C8" t="s">
-        <v>78</v>
-      </c>
-      <c r="D8" t="s">
-        <v>79</v>
-      </c>
-      <c r="E8" t="s">
-        <v>80</v>
-      </c>
-      <c r="J8" s="2">
-        <v>440516</v>
-      </c>
-      <c r="L8" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>113</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>114</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>115</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>118</v>
       </c>
       <c r="E9" t="s">
-        <v>14</v>
-      </c>
-      <c r="J9" s="2">
-        <v>5484169</v>
-      </c>
-      <c r="L9" t="s">
-        <v>130</v>
+        <v>119</v>
+      </c>
+      <c r="F9" t="s">
+        <v>116</v>
+      </c>
+      <c r="G9" t="s">
+        <v>238</v>
+      </c>
+      <c r="H9" t="s">
+        <v>117</v>
+      </c>
+      <c r="I9" t="s">
+        <v>239</v>
+      </c>
+      <c r="J9" s="5">
+        <v>1146</v>
+      </c>
+      <c r="M9" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" t="s">
-        <v>25</v>
-      </c>
-      <c r="J10" s="2">
-        <v>129850798</v>
-      </c>
-      <c r="K10" t="s">
-        <v>26</v>
-      </c>
-      <c r="L10" t="s">
-        <v>23</v>
+      <c r="A10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B10" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" t="s">
-        <v>45</v>
-      </c>
-      <c r="J11" s="2">
-        <v>4604910</v>
-      </c>
-      <c r="L11" t="s">
-        <v>44</v>
+        <v>113</v>
+      </c>
+      <c r="B11" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>0</v>
+        <v>113</v>
       </c>
       <c r="B12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
+        <v>235</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>53</v>
+        <v>113</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
-      </c>
-      <c r="C13" t="s">
-        <v>54</v>
-      </c>
-      <c r="D13" t="s">
-        <v>56</v>
+        <v>236</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>113</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K14" t="s">
-        <v>20</v>
+        <v>237</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>103</v>
+        <v>34</v>
       </c>
       <c r="B15" t="s">
-        <v>107</v>
+        <v>37</v>
       </c>
       <c r="C15" t="s">
-        <v>108</v>
+        <v>35</v>
       </c>
       <c r="D15" t="s">
-        <v>110</v>
+        <v>38</v>
       </c>
       <c r="E15" t="s">
-        <v>111</v>
-      </c>
-      <c r="F15" t="s">
-        <v>112</v>
-      </c>
-      <c r="H15" t="s">
-        <v>106</v>
-      </c>
-      <c r="K15" t="s">
-        <v>109</v>
-      </c>
-      <c r="M15" t="s">
-        <v>104</v>
+        <v>39</v>
+      </c>
+      <c r="J15" s="5">
+        <v>5375469</v>
+      </c>
+      <c r="L15" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>121</v>
+        <v>71</v>
       </c>
       <c r="B16" t="s">
-        <v>123</v>
+        <v>72</v>
       </c>
       <c r="C16" t="s">
-        <v>124</v>
-      </c>
-      <c r="D16" t="s">
-        <v>125</v>
-      </c>
-      <c r="L16" t="s">
-        <v>122</v>
+        <v>73</v>
+      </c>
+      <c r="E16" t="s">
+        <v>74</v>
+      </c>
+      <c r="J16" s="5">
+        <v>56927861</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B17" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C17" t="s">
-        <v>83</v>
+        <v>78</v>
+      </c>
+      <c r="D17" t="s">
+        <v>79</v>
+      </c>
+      <c r="E17" t="s">
+        <v>80</v>
+      </c>
+      <c r="J17" s="5">
+        <v>440516</v>
+      </c>
+      <c r="L17" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>84</v>
+        <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>85</v>
+        <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>86</v>
+        <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>87</v>
+        <v>12</v>
+      </c>
+      <c r="E18" t="s">
+        <v>14</v>
+      </c>
+      <c r="J18" s="5">
+        <v>5484169</v>
+      </c>
+      <c r="L18" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>99</v>
-      </c>
-      <c r="B19" t="s">
-        <v>100</v>
+      <c r="A19" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C19" t="s">
-        <v>101</v>
-      </c>
-      <c r="E19" t="s">
-        <v>102</v>
+        <v>25</v>
+      </c>
+      <c r="J19" s="5">
+        <v>129850798</v>
+      </c>
+      <c r="K19" t="s">
+        <v>26</v>
+      </c>
+      <c r="L19" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>88</v>
-      </c>
-      <c r="B20" t="s">
-        <v>91</v>
+        <v>40</v>
       </c>
       <c r="C20" t="s">
-        <v>90</v>
-      </c>
-      <c r="D20" t="s">
-        <v>92</v>
-      </c>
-      <c r="E20" t="s">
-        <v>93</v>
+        <v>45</v>
+      </c>
+      <c r="J20" s="5">
+        <v>4604910</v>
       </c>
       <c r="L20" t="s">
-        <v>89</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="B21" t="s">
-        <v>67</v>
+        <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>68</v>
-      </c>
-      <c r="E21" t="s">
-        <v>69</v>
-      </c>
-      <c r="M21" t="s">
-        <v>66</v>
+        <v>4</v>
+      </c>
+      <c r="G21" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="B22" t="s">
-        <v>64</v>
-      </c>
-      <c r="C22" t="s">
-        <v>70</v>
-      </c>
-      <c r="L22" t="s">
-        <v>63</v>
+        <v>240</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>126</v>
+        <v>53</v>
       </c>
       <c r="B23" t="s">
-        <v>127</v>
-      </c>
-      <c r="L23" t="s">
-        <v>128</v>
+        <v>55</v>
+      </c>
+      <c r="C23" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" t="s">
+        <v>56</v>
+      </c>
+      <c r="J23" s="5">
+        <v>447765</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>5</v>
-      </c>
-      <c r="M24" t="s">
-        <v>42</v>
+        <v>53</v>
+      </c>
+      <c r="B24" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>6</v>
+        <v>53</v>
+      </c>
+      <c r="B25" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>7</v>
+        <v>53</v>
+      </c>
+      <c r="B26" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>21</v>
+        <v>53</v>
+      </c>
+      <c r="B27" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>15</v>
+      </c>
+      <c r="B28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" t="s">
+        <v>17</v>
+      </c>
+      <c r="J28" s="3">
+        <v>440568</v>
+      </c>
+      <c r="K28" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>103</v>
+      </c>
+      <c r="B29" t="s">
+        <v>107</v>
+      </c>
+      <c r="C29" t="s">
+        <v>108</v>
+      </c>
+      <c r="D29" t="s">
+        <v>110</v>
+      </c>
+      <c r="E29" t="s">
+        <v>111</v>
+      </c>
+      <c r="F29" t="s">
+        <v>112</v>
+      </c>
+      <c r="H29" t="s">
+        <v>106</v>
+      </c>
+      <c r="J29" s="5">
+        <v>129011031</v>
+      </c>
+      <c r="K29" t="s">
+        <v>109</v>
       </c>
       <c r="M29" t="s">
-        <v>43</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>29</v>
-      </c>
-      <c r="M30" t="s">
-        <v>43</v>
+        <v>121</v>
+      </c>
+      <c r="B30" t="s">
+        <v>123</v>
+      </c>
+      <c r="C30" t="s">
+        <v>124</v>
+      </c>
+      <c r="D30" t="s">
+        <v>125</v>
+      </c>
+      <c r="J30" s="5">
+        <v>8376</v>
+      </c>
+      <c r="L30" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>33</v>
-      </c>
-      <c r="M31" t="s">
-        <v>43</v>
+        <v>121</v>
+      </c>
+      <c r="B31" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>46</v>
-      </c>
-      <c r="M32" t="s">
-        <v>47</v>
+        <v>121</v>
+      </c>
+      <c r="B32" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>48</v>
-      </c>
-      <c r="M33" t="s">
-        <v>49</v>
+        <v>81</v>
+      </c>
+      <c r="B33" t="s">
+        <v>82</v>
+      </c>
+      <c r="C33" t="s">
+        <v>83</v>
+      </c>
+      <c r="J33" s="5">
+        <v>56927827</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>57</v>
-      </c>
-      <c r="F34" t="s">
-        <v>59</v>
+        <v>84</v>
+      </c>
+      <c r="B34" t="s">
+        <v>85</v>
+      </c>
+      <c r="C34" t="s">
+        <v>86</v>
+      </c>
+      <c r="D34" t="s">
+        <v>87</v>
+      </c>
+      <c r="J34" s="5">
+        <v>440536</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>60</v>
-      </c>
-      <c r="M35" t="s">
-        <v>61</v>
+        <v>99</v>
+      </c>
+      <c r="B35" t="s">
+        <v>100</v>
+      </c>
+      <c r="C35" t="s">
+        <v>101</v>
+      </c>
+      <c r="E35" t="s">
+        <v>102</v>
+      </c>
+      <c r="J35" s="5">
+        <v>3035516</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>132</v>
+        <v>88</v>
       </c>
       <c r="B36" t="s">
-        <v>137</v>
+        <v>91</v>
       </c>
       <c r="C36" t="s">
-        <v>135</v>
+        <v>90</v>
+      </c>
+      <c r="D36" t="s">
+        <v>92</v>
       </c>
       <c r="E36" t="s">
-        <v>134</v>
-      </c>
-      <c r="F36" t="s">
-        <v>136</v>
-      </c>
-      <c r="H36" t="s">
-        <v>133</v>
+        <v>93</v>
+      </c>
+      <c r="J36" s="5">
+        <v>6054</v>
+      </c>
+      <c r="L36" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>132</v>
+        <v>88</v>
       </c>
       <c r="B37" t="s">
-        <v>138</v>
+        <v>248</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>139</v>
+        <v>88</v>
       </c>
       <c r="B38" t="s">
-        <v>144</v>
-      </c>
-      <c r="C38" t="s">
-        <v>142</v>
-      </c>
-      <c r="E38" t="s">
-        <v>141</v>
-      </c>
-      <c r="F38" t="s">
-        <v>143</v>
-      </c>
-      <c r="H38" t="s">
-        <v>140</v>
+        <v>249</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>139</v>
+        <v>65</v>
       </c>
       <c r="B39" t="s">
-        <v>145</v>
+        <v>67</v>
+      </c>
+      <c r="C39" t="s">
+        <v>68</v>
+      </c>
+      <c r="E39" t="s">
+        <v>69</v>
+      </c>
+      <c r="J39" s="5">
+        <v>124202376</v>
+      </c>
+      <c r="M39" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>146</v>
-      </c>
-      <c r="F40" t="s">
-        <v>59</v>
-      </c>
-      <c r="H40" t="s">
-        <v>147</v>
+        <v>62</v>
+      </c>
+      <c r="B40" t="s">
+        <v>64</v>
+      </c>
+      <c r="C40" t="s">
+        <v>70</v>
+      </c>
+      <c r="G40" t="s">
+        <v>250</v>
+      </c>
+      <c r="J40" s="5">
+        <v>6991982</v>
+      </c>
+      <c r="L40" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>148</v>
-      </c>
-      <c r="H41" t="s">
-        <v>149</v>
+        <v>126</v>
+      </c>
+      <c r="B41" t="s">
+        <v>127</v>
+      </c>
+      <c r="L41" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>150</v>
-      </c>
-      <c r="B42" t="s">
-        <v>155</v>
-      </c>
-      <c r="C42" t="s">
-        <v>153</v>
-      </c>
-      <c r="E42" t="s">
-        <v>152</v>
-      </c>
-      <c r="F42" t="s">
-        <v>154</v>
-      </c>
-      <c r="H42" t="s">
-        <v>151</v>
+        <v>5</v>
+      </c>
+      <c r="M42" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>150</v>
-      </c>
-      <c r="B43" t="s">
-        <v>156</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>157</v>
-      </c>
-      <c r="B44" t="s">
-        <v>162</v>
-      </c>
-      <c r="C44" t="s">
-        <v>160</v>
-      </c>
-      <c r="E44" t="s">
-        <v>159</v>
-      </c>
-      <c r="F44" t="s">
-        <v>161</v>
-      </c>
-      <c r="H44" t="s">
-        <v>158</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>157</v>
-      </c>
-      <c r="B45" t="s">
-        <v>163</v>
+        <v>21</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>164</v>
-      </c>
-      <c r="B46" t="s">
-        <v>169</v>
-      </c>
-      <c r="C46" t="s">
-        <v>167</v>
-      </c>
-      <c r="D46" t="s">
-        <v>174</v>
-      </c>
-      <c r="E46" t="s">
-        <v>166</v>
-      </c>
-      <c r="F46" t="s">
-        <v>168</v>
-      </c>
-      <c r="G46" t="s">
-        <v>176</v>
-      </c>
-      <c r="H46" t="s">
-        <v>165</v>
+        <v>27</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>164</v>
-      </c>
-      <c r="B47" t="s">
-        <v>170</v>
-      </c>
-      <c r="G47" t="s">
-        <v>177</v>
+        <v>28</v>
+      </c>
+      <c r="M47" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>29</v>
+      </c>
+      <c r="M48" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>33</v>
+      </c>
+      <c r="M49" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>46</v>
+      </c>
+      <c r="M50" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>48</v>
+      </c>
+      <c r="M51" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>57</v>
+      </c>
+      <c r="F52" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>60</v>
+      </c>
+      <c r="M53" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>132</v>
+      </c>
+      <c r="B54" t="s">
+        <v>137</v>
+      </c>
+      <c r="C54" t="s">
+        <v>135</v>
+      </c>
+      <c r="E54" t="s">
+        <v>134</v>
+      </c>
+      <c r="F54" t="s">
+        <v>136</v>
+      </c>
+      <c r="H54" t="s">
+        <v>133</v>
+      </c>
+      <c r="J54" s="5">
+        <v>123935</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>132</v>
+      </c>
+      <c r="B55" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>139</v>
+      </c>
+      <c r="B56" t="s">
+        <v>144</v>
+      </c>
+      <c r="C56" t="s">
+        <v>142</v>
+      </c>
+      <c r="E56" t="s">
+        <v>141</v>
+      </c>
+      <c r="F56" t="s">
+        <v>143</v>
+      </c>
+      <c r="H56" t="s">
+        <v>140</v>
+      </c>
+      <c r="J56" s="5">
+        <v>123913</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>139</v>
+      </c>
+      <c r="B57" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>146</v>
+      </c>
+      <c r="F58" t="s">
+        <v>59</v>
+      </c>
+      <c r="H58" t="s">
+        <v>147</v>
+      </c>
+      <c r="J58" s="5">
+        <v>6427004</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>148</v>
+      </c>
+      <c r="H59" t="s">
+        <v>149</v>
+      </c>
+      <c r="J59" s="5">
+        <v>9837455</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>150</v>
+      </c>
+      <c r="B60" t="s">
+        <v>155</v>
+      </c>
+      <c r="C60" t="s">
+        <v>153</v>
+      </c>
+      <c r="E60" t="s">
+        <v>152</v>
+      </c>
+      <c r="F60" t="s">
+        <v>154</v>
+      </c>
+      <c r="H60" t="s">
+        <v>151</v>
+      </c>
+      <c r="J60" s="5">
+        <v>96801</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>150</v>
+      </c>
+      <c r="B61" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>157</v>
+      </c>
+      <c r="B62" t="s">
+        <v>162</v>
+      </c>
+      <c r="C62" t="s">
+        <v>160</v>
+      </c>
+      <c r="E62" t="s">
+        <v>159</v>
+      </c>
+      <c r="F62" t="s">
+        <v>161</v>
+      </c>
+      <c r="H62" t="s">
+        <v>158</v>
+      </c>
+      <c r="J62" s="5">
+        <v>6998029</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>157</v>
+      </c>
+      <c r="B63" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
         <v>164</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B64" t="s">
+        <v>169</v>
+      </c>
+      <c r="C64" t="s">
+        <v>167</v>
+      </c>
+      <c r="D64" t="s">
+        <v>174</v>
+      </c>
+      <c r="E64" t="s">
+        <v>166</v>
+      </c>
+      <c r="F64" t="s">
+        <v>168</v>
+      </c>
+      <c r="G64" t="s">
+        <v>176</v>
+      </c>
+      <c r="H64" t="s">
+        <v>165</v>
+      </c>
+      <c r="J64" s="5">
+        <v>2879</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>164</v>
+      </c>
+      <c r="B65" t="s">
+        <v>170</v>
+      </c>
+      <c r="G65" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>164</v>
+      </c>
+      <c r="B66" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
         <v>164</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B67" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
         <v>164</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B68" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
         <v>178</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B69" t="s">
         <v>185</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C69" t="s">
         <v>181</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D69" t="s">
         <v>190</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E69" t="s">
         <v>180</v>
       </c>
-      <c r="F51" t="s">
+      <c r="F69" t="s">
         <v>182</v>
       </c>
-      <c r="G51" t="s">
+      <c r="G69" t="s">
         <v>191</v>
       </c>
-      <c r="H51" t="s">
+      <c r="H69" t="s">
         <v>179</v>
       </c>
-      <c r="I51" t="s">
+      <c r="I69" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+      <c r="J69" s="5">
+        <v>440018</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
         <v>178</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B70" t="s">
         <v>186</v>
       </c>
-      <c r="G52" t="s">
+      <c r="G70" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
         <v>178</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B71" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
         <v>178</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B72" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
         <v>178</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B73" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
         <v>193</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B74" t="s">
         <v>195</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C74" t="s">
         <v>194</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D74" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+      <c r="J74" s="5">
+        <v>5281976</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
         <v>193</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B75" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
         <v>193</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B76" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
         <v>199</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B77" t="s">
         <v>203</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C77" t="s">
         <v>201</v>
       </c>
-      <c r="F59" t="s">
+      <c r="F77" t="s">
         <v>202</v>
       </c>
-      <c r="G59" t="s">
+      <c r="G77" t="s">
         <v>205</v>
       </c>
-      <c r="H59" t="s">
+      <c r="H77" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+      <c r="J77" s="5">
+        <v>92953</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
         <v>199</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B78" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
         <v>206</v>
       </c>
-      <c r="H61" t="s">
+      <c r="H79" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
+      <c r="J79" s="5">
+        <v>92829</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
         <v>208</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B80" t="s">
         <v>212</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C80" t="s">
         <v>210</v>
       </c>
-      <c r="E62" t="s">
+      <c r="E80" t="s">
         <v>214</v>
       </c>
-      <c r="F62" t="s">
+      <c r="F80" t="s">
         <v>211</v>
       </c>
-      <c r="H62" t="s">
+      <c r="H80" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
+      <c r="J80" s="5">
+        <v>151282</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
         <v>208</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B81" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
         <v>215</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B82" t="s">
         <v>220</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C82" t="s">
         <v>217</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D82" t="s">
         <v>222</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E82" t="s">
         <v>223</v>
       </c>
-      <c r="F64" t="s">
+      <c r="F82" t="s">
         <v>218</v>
       </c>
-      <c r="G64" t="s">
+      <c r="G82" t="s">
         <v>221</v>
       </c>
-      <c r="H64" t="s">
+      <c r="H82" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
+      <c r="J82" s="5">
+        <v>92843</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
         <v>215</v>
       </c>
-      <c r="F65" t="s">
+      <c r="F83" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
         <v>224</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B84" t="s">
         <v>228</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C84" t="s">
         <v>226</v>
       </c>
-      <c r="F66" t="s">
+      <c r="F84" t="s">
         <v>227</v>
       </c>
-      <c r="H66" t="s">
+      <c r="H84" t="s">
         <v>225</v>
       </c>
+      <c r="J84" s="5">
+        <v>7408690</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M35">
-    <sortCondition ref="C2:C35"/>
-    <sortCondition ref="B2:B35"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:M53">
+    <sortCondition ref="C6:C53"/>
+    <sortCondition ref="B6:B53"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[CORR] add P.putida into data
</commit_message>
<xml_diff>
--- a/data/manual_annotations.xlsx
+++ b/data/manual_annotations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/baeuerle/Organisation/Masterarbeit/C_striatum_GEMs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDC9153D-03F8-5F4B-B97A-5A34B428E6AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5CC06CC-F5BE-B94D-8CFE-58336DAE6C6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33600" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{8C7181AF-021E-984D-A4FD-BACD10035A87}"/>
+    <workbookView xWindow="-31540" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{8C7181AF-021E-984D-A4FD-BACD10035A87}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>

</xml_diff>